<commit_message>
Update of the error message
</commit_message>
<xml_diff>
--- a/Classes Lifecicle.xlsx
+++ b/Classes Lifecicle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ANANAS\Projects\Visual Studio Projects\DemoBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hubva\Documents\Visual Studio 2019\DemoBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA02F2D3-D2D3-4B52-93D9-1BA549710A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C5AA6E-FB25-44E7-ADB1-E372629D0062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="948" windowWidth="17676" windowHeight="10284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12372" yWindow="-14508" windowWidth="20460" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -121,8 +121,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,13 +158,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,7 +452,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,10 +465,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>